<commit_message>
Update Generic example data inputs
</commit_message>
<xml_diff>
--- a/example_data/example_preprocessed_annotation.xlsx
+++ b/example_data/example_preprocessed_annotation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gracerhpotter/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gracerhpotter/Documents/EmiliLab/OmNI/example_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57F26E11-CA4D-DF48-9B1F-39EB6DFD1913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09DA3502-9C2F-9A48-B858-DE9F82BB136D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Inputs" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="42">
   <si>
     <t>Omics Notebook Annotation File</t>
   </si>
@@ -333,12 +333,6 @@
     <t>example_preprocessed.txt</t>
   </si>
   <si>
-    <t>PreFormattedData</t>
-  </si>
-  <si>
-    <t>PreFormatted</t>
-  </si>
-  <si>
     <t>Group</t>
   </si>
   <si>
@@ -357,9 +351,6 @@
     <t>Glucose5</t>
   </si>
   <si>
-    <t>Glucose6</t>
-  </si>
-  <si>
     <t>NoGlucose1</t>
   </si>
   <si>
@@ -375,13 +366,16 @@
     <t>NoGlucose5</t>
   </si>
   <si>
-    <t>NoGlucose6</t>
-  </si>
-  <si>
     <t>Glucose</t>
   </si>
   <si>
     <t>NoGlucose</t>
+  </si>
+  <si>
+    <t>Generic</t>
+  </si>
+  <si>
+    <t>PreProcessedData</t>
   </si>
 </sst>
 </file>
@@ -1017,20 +1011,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1052,28 +1047,27 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1295,7 +1289,7 @@
   <dimension ref="A1:Z1008"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1306,10 +1300,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32"/>
+      <c r="B1" s="33"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="2"/>
@@ -1336,8 +1330,8 @@
       <c r="Z1" s="2"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="34"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="35"/>
       <c r="C2" s="1"/>
       <c r="D2" s="1"/>
       <c r="E2" s="2"/>
@@ -1363,20 +1357,20 @@
       <c r="Y2" s="2"/>
       <c r="Z2" s="2"/>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" s="35" t="s">
+    <row r="3" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="36"/>
+      <c r="B3" s="37"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
-      <c r="E3" s="40" t="s">
+      <c r="E3" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="41"/>
-      <c r="G3" s="41"/>
-      <c r="H3" s="41"/>
-      <c r="I3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+      <c r="H3" s="42"/>
+      <c r="I3" s="43"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
@@ -1395,16 +1389,16 @@
       <c r="Y3" s="2"/>
       <c r="Z3" s="2"/>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A4" s="37"/>
-      <c r="B4" s="36"/>
+    <row r="4" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="A4" s="38"/>
+      <c r="B4" s="37"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
-      <c r="E4" s="43"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="H4" s="44"/>
-      <c r="I4" s="45"/>
+      <c r="E4" s="44"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="46"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
@@ -1423,18 +1417,18 @@
       <c r="Y4" s="2"/>
       <c r="Z4" s="2"/>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A5" s="38"/>
-      <c r="B5" s="39"/>
+    <row r="5" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="39"/>
+      <c r="B5" s="40"/>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="47"/>
+      <c r="F5" s="26"/>
+      <c r="G5" s="26"/>
+      <c r="H5" s="26"/>
+      <c r="I5" s="27"/>
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
@@ -1453,20 +1447,20 @@
       <c r="Y5" s="2"/>
       <c r="Z5" s="2"/>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="48" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="23"/>
+      <c r="B6" s="26"/>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
-      <c r="E6" s="49" t="s">
+      <c r="E6" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="47"/>
+      <c r="F6" s="26"/>
+      <c r="G6" s="26"/>
+      <c r="H6" s="26"/>
+      <c r="I6" s="27"/>
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
@@ -1485,16 +1479,16 @@
       <c r="Y6" s="2"/>
       <c r="Z6" s="2"/>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23"/>
+    <row r="7" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="26"/>
+      <c r="B7" s="26"/>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="50"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="47"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="26"/>
+      <c r="G7" s="26"/>
+      <c r="H7" s="26"/>
+      <c r="I7" s="27"/>
       <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
@@ -1513,18 +1507,18 @@
       <c r="Y7" s="2"/>
       <c r="Z7" s="2"/>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
+    <row r="8" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="49"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="49" t="s">
+      <c r="E8" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
-      <c r="I8" s="47"/>
+      <c r="F8" s="26"/>
+      <c r="G8" s="26"/>
+      <c r="H8" s="26"/>
+      <c r="I8" s="27"/>
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
       <c r="L8" s="2"/>
@@ -1543,16 +1537,16 @@
       <c r="Y8" s="2"/>
       <c r="Z8" s="2"/>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
+    <row r="9" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="26"/>
+      <c r="B9" s="26"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="50"/>
-      <c r="F9" s="23"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="23"/>
-      <c r="I9" s="47"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="26"/>
+      <c r="G9" s="26"/>
+      <c r="H9" s="26"/>
+      <c r="I9" s="27"/>
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
       <c r="L9" s="2"/>
@@ -1571,20 +1565,20 @@
       <c r="Y9" s="2"/>
       <c r="Z9" s="2"/>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A10" s="24" t="s">
+    <row r="10" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="53" t="s">
         <v>8</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="50"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="23"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="47"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="26"/>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="27"/>
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
       <c r="L10" s="2"/>
@@ -1603,18 +1597,18 @@
       <c r="Y10" s="2"/>
       <c r="Z10" s="2"/>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A11" s="25"/>
-      <c r="B11" s="28"/>
+    <row r="11" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="51"/>
+      <c r="B11" s="54"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="58" t="s">
+      <c r="E11" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="53"/>
-      <c r="G11" s="53"/>
-      <c r="H11" s="53"/>
-      <c r="I11" s="54"/>
+      <c r="F11" s="23"/>
+      <c r="G11" s="23"/>
+      <c r="H11" s="23"/>
+      <c r="I11" s="24"/>
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
       <c r="L11" s="2"/>
@@ -1633,18 +1627,18 @@
       <c r="Y11" s="2"/>
       <c r="Z11" s="2"/>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A12" s="25"/>
-      <c r="B12" s="28"/>
+    <row r="12" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="51"/>
+      <c r="B12" s="54"/>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="49" t="s">
+      <c r="E12" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="F12" s="23"/>
-      <c r="G12" s="23"/>
-      <c r="H12" s="23"/>
-      <c r="I12" s="47"/>
+      <c r="F12" s="26"/>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="27"/>
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
       <c r="L12" s="2"/>
@@ -1663,16 +1657,16 @@
       <c r="Y12" s="2"/>
       <c r="Z12" s="2"/>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A13" s="25"/>
-      <c r="B13" s="28"/>
+    <row r="13" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="51"/>
+      <c r="B13" s="54"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="50"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="23"/>
-      <c r="H13" s="23"/>
-      <c r="I13" s="47"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="27"/>
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
       <c r="L13" s="2"/>
@@ -1691,18 +1685,18 @@
       <c r="Y13" s="2"/>
       <c r="Z13" s="2"/>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A14" s="25"/>
-      <c r="B14" s="28"/>
+    <row r="14" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="51"/>
+      <c r="B14" s="54"/>
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="49" t="s">
+      <c r="E14" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="F14" s="23"/>
-      <c r="G14" s="23"/>
-      <c r="H14" s="23"/>
-      <c r="I14" s="47"/>
+      <c r="F14" s="26"/>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="27"/>
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
       <c r="L14" s="2"/>
@@ -1721,16 +1715,16 @@
       <c r="Y14" s="2"/>
       <c r="Z14" s="2"/>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A15" s="26"/>
-      <c r="B15" s="29"/>
+    <row r="15" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="52"/>
+      <c r="B15" s="55"/>
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="50"/>
-      <c r="F15" s="23"/>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
-      <c r="I15" s="47"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="26"/>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="27"/>
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
       <c r="L15" s="2"/>
@@ -1749,7 +1743,7 @@
       <c r="Y15" s="2"/>
       <c r="Z15" s="2"/>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:26" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>12</v>
       </c>
@@ -1760,11 +1754,11 @@
         <v>14</v>
       </c>
       <c r="D16" s="4"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="23"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="47"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="26"/>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="27"/>
       <c r="J16" s="8"/>
       <c r="K16" s="8"/>
       <c r="L16" s="8"/>
@@ -1788,19 +1782,19 @@
         <v>26</v>
       </c>
       <c r="B17" s="10" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>28</v>
+        <v>40</v>
       </c>
       <c r="D17" s="4"/>
-      <c r="E17" s="59" t="s">
+      <c r="E17" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="F17" s="23"/>
-      <c r="G17" s="23"/>
-      <c r="H17" s="23"/>
-      <c r="I17" s="47"/>
+      <c r="F17" s="26"/>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="27"/>
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
       <c r="L17" s="2"/>
@@ -1819,16 +1813,16 @@
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="9"/>
       <c r="B18" s="10"/>
       <c r="C18" s="11"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="50"/>
-      <c r="F18" s="23"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="23"/>
-      <c r="I18" s="47"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="26"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="27"/>
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
@@ -1847,16 +1841,16 @@
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="9"/>
       <c r="B19" s="10"/>
       <c r="C19" s="12"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="23"/>
-      <c r="G19" s="23"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="47"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="26"/>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="27"/>
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
@@ -1875,16 +1869,16 @@
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" s="9"/>
       <c r="B20" s="10"/>
       <c r="C20" s="12"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="50"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="47"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="26"/>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="27"/>
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
@@ -1903,18 +1897,18 @@
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" s="9"/>
       <c r="B21" s="10"/>
       <c r="C21" s="12"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="49" t="s">
+      <c r="E21" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="F21" s="23"/>
-      <c r="G21" s="23"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="47"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="27"/>
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
@@ -1933,16 +1927,16 @@
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" s="9"/>
       <c r="B22" s="10"/>
       <c r="C22" s="12"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="23"/>
-      <c r="G22" s="23"/>
-      <c r="H22" s="23"/>
-      <c r="I22" s="47"/>
+      <c r="E22" s="28"/>
+      <c r="F22" s="26"/>
+      <c r="G22" s="26"/>
+      <c r="H22" s="26"/>
+      <c r="I22" s="27"/>
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
@@ -1961,16 +1955,16 @@
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="9"/>
       <c r="B23" s="10"/>
       <c r="C23" s="12"/>
       <c r="D23" s="2"/>
-      <c r="E23" s="50"/>
-      <c r="F23" s="23"/>
-      <c r="G23" s="23"/>
-      <c r="H23" s="23"/>
-      <c r="I23" s="47"/>
+      <c r="E23" s="28"/>
+      <c r="F23" s="26"/>
+      <c r="G23" s="26"/>
+      <c r="H23" s="26"/>
+      <c r="I23" s="27"/>
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
@@ -1989,16 +1983,16 @@
       <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="9"/>
       <c r="B24" s="10"/>
       <c r="C24" s="12"/>
       <c r="D24" s="2"/>
-      <c r="E24" s="50"/>
-      <c r="F24" s="23"/>
-      <c r="G24" s="23"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="47"/>
+      <c r="E24" s="28"/>
+      <c r="F24" s="26"/>
+      <c r="G24" s="26"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="27"/>
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
@@ -2017,16 +2011,16 @@
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" s="9"/>
       <c r="B25" s="10"/>
       <c r="C25" s="12"/>
       <c r="D25" s="2"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="23"/>
-      <c r="G25" s="23"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="47"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="26"/>
+      <c r="G25" s="26"/>
+      <c r="H25" s="26"/>
+      <c r="I25" s="27"/>
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
@@ -2045,16 +2039,16 @@
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
     </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="9"/>
       <c r="B26" s="10"/>
       <c r="C26" s="12"/>
       <c r="D26" s="2"/>
-      <c r="E26" s="50"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="23"/>
-      <c r="I26" s="47"/>
+      <c r="E26" s="28"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="27"/>
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
@@ -2073,18 +2067,18 @@
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
     </row>
-    <row r="27" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" s="9"/>
       <c r="B27" s="10"/>
       <c r="C27" s="12"/>
       <c r="D27" s="2"/>
-      <c r="E27" s="60" t="s">
+      <c r="E27" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="F27" s="53"/>
-      <c r="G27" s="53"/>
-      <c r="H27" s="53"/>
-      <c r="I27" s="54"/>
+      <c r="F27" s="23"/>
+      <c r="G27" s="23"/>
+      <c r="H27" s="23"/>
+      <c r="I27" s="24"/>
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
@@ -2103,18 +2097,18 @@
       <c r="Y27" s="2"/>
       <c r="Z27" s="2"/>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" s="9"/>
       <c r="B28" s="10"/>
       <c r="C28" s="12"/>
       <c r="D28" s="2"/>
-      <c r="E28" s="49" t="s">
+      <c r="E28" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="F28" s="23"/>
-      <c r="G28" s="23"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="47"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="27"/>
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
@@ -2133,16 +2127,16 @@
       <c r="Y28" s="2"/>
       <c r="Z28" s="2"/>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="9"/>
       <c r="B29" s="10"/>
       <c r="C29" s="12"/>
       <c r="D29" s="2"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="23"/>
-      <c r="H29" s="23"/>
-      <c r="I29" s="47"/>
+      <c r="E29" s="28"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="27"/>
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
@@ -2161,16 +2155,16 @@
       <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="9"/>
       <c r="B30" s="10"/>
       <c r="C30" s="12"/>
       <c r="D30" s="2"/>
-      <c r="E30" s="50"/>
-      <c r="F30" s="23"/>
-      <c r="G30" s="23"/>
-      <c r="H30" s="23"/>
-      <c r="I30" s="47"/>
+      <c r="E30" s="28"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="27"/>
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
@@ -2189,18 +2183,18 @@
       <c r="Y30" s="2"/>
       <c r="Z30" s="2"/>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" s="9"/>
       <c r="B31" s="10"/>
       <c r="C31" s="12"/>
       <c r="D31" s="2"/>
-      <c r="E31" s="49" t="s">
+      <c r="E31" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="F31" s="23"/>
-      <c r="G31" s="23"/>
-      <c r="H31" s="23"/>
-      <c r="I31" s="47"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="27"/>
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
@@ -2219,16 +2213,16 @@
       <c r="Y31" s="2"/>
       <c r="Z31" s="2"/>
     </row>
-    <row r="32" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="9"/>
       <c r="B32" s="10"/>
       <c r="C32" s="12"/>
       <c r="D32" s="2"/>
-      <c r="E32" s="50"/>
-      <c r="F32" s="23"/>
-      <c r="G32" s="23"/>
-      <c r="H32" s="23"/>
-      <c r="I32" s="47"/>
+      <c r="E32" s="28"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="27"/>
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
@@ -2247,18 +2241,18 @@
       <c r="Y32" s="2"/>
       <c r="Z32" s="2"/>
     </row>
-    <row r="33" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="9"/>
       <c r="B33" s="10"/>
       <c r="C33" s="12"/>
       <c r="D33" s="2"/>
-      <c r="E33" s="51" t="s">
+      <c r="E33" s="56" t="s">
         <v>20</v>
       </c>
-      <c r="F33" s="23"/>
-      <c r="G33" s="23"/>
-      <c r="H33" s="23"/>
-      <c r="I33" s="47"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="27"/>
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
@@ -2277,18 +2271,18 @@
       <c r="Y33" s="2"/>
       <c r="Z33" s="2"/>
     </row>
-    <row r="34" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" s="9"/>
       <c r="B34" s="10"/>
       <c r="C34" s="12"/>
       <c r="D34" s="2"/>
-      <c r="E34" s="51" t="s">
+      <c r="E34" s="56" t="s">
         <v>21</v>
       </c>
-      <c r="F34" s="23"/>
-      <c r="G34" s="23"/>
-      <c r="H34" s="23"/>
-      <c r="I34" s="47"/>
+      <c r="F34" s="26"/>
+      <c r="G34" s="26"/>
+      <c r="H34" s="26"/>
+      <c r="I34" s="27"/>
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
@@ -2307,18 +2301,18 @@
       <c r="Y34" s="2"/>
       <c r="Z34" s="2"/>
     </row>
-    <row r="35" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" s="9"/>
       <c r="B35" s="10"/>
       <c r="C35" s="12"/>
       <c r="D35" s="2"/>
-      <c r="E35" s="52" t="s">
+      <c r="E35" s="57" t="s">
         <v>22</v>
       </c>
-      <c r="F35" s="53"/>
-      <c r="G35" s="53"/>
-      <c r="H35" s="53"/>
-      <c r="I35" s="54"/>
+      <c r="F35" s="23"/>
+      <c r="G35" s="23"/>
+      <c r="H35" s="23"/>
+      <c r="I35" s="24"/>
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
@@ -2337,18 +2331,18 @@
       <c r="Y35" s="2"/>
       <c r="Z35" s="2"/>
     </row>
-    <row r="36" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" s="9"/>
       <c r="B36" s="10"/>
       <c r="C36" s="12"/>
       <c r="D36" s="2"/>
-      <c r="E36" s="49" t="s">
+      <c r="E36" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="F36" s="23"/>
-      <c r="G36" s="23"/>
-      <c r="H36" s="23"/>
-      <c r="I36" s="47"/>
+      <c r="F36" s="26"/>
+      <c r="G36" s="26"/>
+      <c r="H36" s="26"/>
+      <c r="I36" s="27"/>
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
@@ -2367,16 +2361,16 @@
       <c r="Y36" s="2"/>
       <c r="Z36" s="2"/>
     </row>
-    <row r="37" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" s="9"/>
       <c r="B37" s="10"/>
       <c r="C37" s="12"/>
       <c r="D37" s="2"/>
-      <c r="E37" s="55"/>
-      <c r="F37" s="56"/>
-      <c r="G37" s="56"/>
-      <c r="H37" s="56"/>
-      <c r="I37" s="57"/>
+      <c r="E37" s="58"/>
+      <c r="F37" s="59"/>
+      <c r="G37" s="59"/>
+      <c r="H37" s="59"/>
+      <c r="I37" s="60"/>
       <c r="J37" s="2"/>
       <c r="K37" s="2"/>
       <c r="L37" s="2"/>
@@ -2395,7 +2389,7 @@
       <c r="Y37" s="2"/>
       <c r="Z37" s="2"/>
     </row>
-    <row r="38" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="9"/>
       <c r="B38" s="10"/>
       <c r="C38" s="12"/>
@@ -2423,7 +2417,7 @@
       <c r="Y38" s="2"/>
       <c r="Z38" s="2"/>
     </row>
-    <row r="39" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="9"/>
       <c r="B39" s="10"/>
       <c r="C39" s="12"/>
@@ -2451,7 +2445,7 @@
       <c r="Y39" s="2"/>
       <c r="Z39" s="2"/>
     </row>
-    <row r="40" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="9"/>
       <c r="B40" s="10"/>
       <c r="C40" s="12"/>
@@ -2479,7 +2473,7 @@
       <c r="Y40" s="2"/>
       <c r="Z40" s="2"/>
     </row>
-    <row r="41" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" s="9"/>
       <c r="B41" s="10"/>
       <c r="C41" s="12"/>
@@ -2507,7 +2501,7 @@
       <c r="Y41" s="2"/>
       <c r="Z41" s="2"/>
     </row>
-    <row r="42" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="9"/>
       <c r="B42" s="10"/>
       <c r="C42" s="12"/>
@@ -2535,7 +2529,7 @@
       <c r="Y42" s="2"/>
       <c r="Z42" s="2"/>
     </row>
-    <row r="43" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" s="9"/>
       <c r="B43" s="10"/>
       <c r="C43" s="12"/>
@@ -2563,7 +2557,7 @@
       <c r="Y43" s="2"/>
       <c r="Z43" s="2"/>
     </row>
-    <row r="44" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" s="9"/>
       <c r="B44" s="10"/>
       <c r="C44" s="12"/>
@@ -2591,7 +2585,7 @@
       <c r="Y44" s="2"/>
       <c r="Z44" s="2"/>
     </row>
-    <row r="45" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="9"/>
       <c r="B45" s="10"/>
       <c r="C45" s="12"/>
@@ -2619,7 +2613,7 @@
       <c r="Y45" s="2"/>
       <c r="Z45" s="2"/>
     </row>
-    <row r="46" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="9"/>
       <c r="B46" s="10"/>
       <c r="C46" s="12"/>
@@ -2647,7 +2641,7 @@
       <c r="Y46" s="2"/>
       <c r="Z46" s="2"/>
     </row>
-    <row r="47" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="9"/>
       <c r="B47" s="10"/>
       <c r="C47" s="12"/>
@@ -2675,7 +2669,7 @@
       <c r="Y47" s="2"/>
       <c r="Z47" s="2"/>
     </row>
-    <row r="48" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="9"/>
       <c r="B48" s="10"/>
       <c r="C48" s="12"/>
@@ -2703,7 +2697,7 @@
       <c r="Y48" s="2"/>
       <c r="Z48" s="2"/>
     </row>
-    <row r="49" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="9"/>
       <c r="B49" s="10"/>
       <c r="C49" s="12"/>
@@ -2731,7 +2725,7 @@
       <c r="Y49" s="2"/>
       <c r="Z49" s="2"/>
     </row>
-    <row r="50" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="9"/>
       <c r="B50" s="10"/>
       <c r="C50" s="12"/>
@@ -2759,7 +2753,7 @@
       <c r="Y50" s="2"/>
       <c r="Z50" s="2"/>
     </row>
-    <row r="51" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="9"/>
       <c r="B51" s="10"/>
       <c r="C51" s="12"/>
@@ -2787,7 +2781,7 @@
       <c r="Y51" s="2"/>
       <c r="Z51" s="2"/>
     </row>
-    <row r="52" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" s="9"/>
       <c r="B52" s="10"/>
       <c r="C52" s="12"/>
@@ -2815,7 +2809,7 @@
       <c r="Y52" s="2"/>
       <c r="Z52" s="2"/>
     </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="9"/>
       <c r="B53" s="10"/>
       <c r="C53" s="12"/>
@@ -2843,7 +2837,7 @@
       <c r="Y53" s="2"/>
       <c r="Z53" s="2"/>
     </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="9"/>
       <c r="B54" s="10"/>
       <c r="C54" s="12"/>
@@ -2871,7 +2865,7 @@
       <c r="Y54" s="2"/>
       <c r="Z54" s="2"/>
     </row>
-    <row r="55" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="9"/>
       <c r="B55" s="10"/>
       <c r="C55" s="12"/>
@@ -2899,7 +2893,7 @@
       <c r="Y55" s="2"/>
       <c r="Z55" s="2"/>
     </row>
-    <row r="56" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="9"/>
       <c r="B56" s="10"/>
       <c r="C56" s="12"/>
@@ -2927,7 +2921,7 @@
       <c r="Y56" s="2"/>
       <c r="Z56" s="2"/>
     </row>
-    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="13"/>
       <c r="B57" s="14"/>
       <c r="C57" s="15"/>
@@ -2955,11 +2949,11 @@
       <c r="Y57" s="2"/>
       <c r="Z57" s="2"/>
     </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A58" s="30" t="s">
+    <row r="58" spans="1:26" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B58" s="23"/>
+      <c r="B58" s="26"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -2985,7 +2979,7 @@
       <c r="Y58" s="2"/>
       <c r="Z58" s="2"/>
     </row>
-    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="2"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -3013,7 +3007,7 @@
       <c r="Y59" s="2"/>
       <c r="Z59" s="2"/>
     </row>
-    <row r="60" spans="1:26" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:26" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="2"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -29587,18 +29581,9 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="E27:I27"/>
-    <mergeCell ref="E28:I30"/>
-    <mergeCell ref="E11:I11"/>
-    <mergeCell ref="E12:I13"/>
-    <mergeCell ref="E14:I16"/>
-    <mergeCell ref="E17:I20"/>
-    <mergeCell ref="E21:I26"/>
-    <mergeCell ref="E31:I32"/>
-    <mergeCell ref="E33:I33"/>
-    <mergeCell ref="E34:I34"/>
-    <mergeCell ref="E35:I35"/>
-    <mergeCell ref="E36:I37"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="A1:B2"/>
+    <mergeCell ref="A3:B5"/>
     <mergeCell ref="E3:I4"/>
     <mergeCell ref="E5:I5"/>
     <mergeCell ref="A6:B7"/>
@@ -29607,9 +29592,18 @@
     <mergeCell ref="A8:B9"/>
     <mergeCell ref="A10:A15"/>
     <mergeCell ref="B10:B15"/>
-    <mergeCell ref="A58:B58"/>
-    <mergeCell ref="A1:B2"/>
-    <mergeCell ref="A3:B5"/>
+    <mergeCell ref="E31:I32"/>
+    <mergeCell ref="E33:I33"/>
+    <mergeCell ref="E34:I34"/>
+    <mergeCell ref="E35:I35"/>
+    <mergeCell ref="E36:I37"/>
+    <mergeCell ref="E27:I27"/>
+    <mergeCell ref="E28:I30"/>
+    <mergeCell ref="E11:I11"/>
+    <mergeCell ref="E12:I13"/>
+    <mergeCell ref="E14:I16"/>
+    <mergeCell ref="E17:I20"/>
+    <mergeCell ref="E21:I26"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C17:C57" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -29625,11 +29619,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z1000"/>
+  <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12:XFD12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -29646,10 +29640,10 @@
       </c>
       <c r="B1" s="17" t="str">
         <f>IF(Inputs!B17&lt;&gt;"",Inputs!B17,"")</f>
-        <v>PreFormattedData</v>
+        <v>PreProcessedData</v>
       </c>
       <c r="C1" s="18" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D1" s="17" t="str">
         <f>IF(Inputs!B19&lt;&gt;"",Inputs!B19,"")</f>
@@ -29692,13 +29686,13 @@
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D2" s="10"/>
       <c r="E2" s="10"/>
@@ -29726,13 +29720,13 @@
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D3" s="10"/>
       <c r="E3" s="10"/>
@@ -29760,13 +29754,13 @@
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D4" s="10"/>
       <c r="E4" s="10"/>
@@ -29794,13 +29788,13 @@
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D5" s="10"/>
       <c r="E5" s="10"/>
@@ -29828,13 +29822,13 @@
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A6" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="D6" s="10"/>
       <c r="E6" s="10"/>
@@ -29862,13 +29856,13 @@
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A7" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
@@ -29896,13 +29890,13 @@
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
@@ -29930,13 +29924,13 @@
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A9" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -29964,13 +29958,13 @@
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A10" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -29998,13 +29992,13 @@
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -30031,15 +30025,9 @@
       <c r="Z11" s="21"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="A12" s="20"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -30065,15 +30053,9 @@
       <c r="Z12" s="21"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>43</v>
-      </c>
+      <c r="A13" s="20"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -57678,62 +57660,6 @@
       <c r="Y998" s="10"/>
       <c r="Z998" s="21"/>
     </row>
-    <row r="999" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A999" s="20"/>
-      <c r="B999" s="10"/>
-      <c r="C999" s="10"/>
-      <c r="D999" s="10"/>
-      <c r="E999" s="10"/>
-      <c r="F999" s="10"/>
-      <c r="G999" s="10"/>
-      <c r="H999" s="10"/>
-      <c r="I999" s="10"/>
-      <c r="J999" s="10"/>
-      <c r="K999" s="10"/>
-      <c r="L999" s="10"/>
-      <c r="M999" s="10"/>
-      <c r="N999" s="10"/>
-      <c r="O999" s="10"/>
-      <c r="P999" s="10"/>
-      <c r="Q999" s="10"/>
-      <c r="R999" s="10"/>
-      <c r="S999" s="10"/>
-      <c r="T999" s="10"/>
-      <c r="U999" s="10"/>
-      <c r="V999" s="10"/>
-      <c r="W999" s="10"/>
-      <c r="X999" s="10"/>
-      <c r="Y999" s="10"/>
-      <c r="Z999" s="21"/>
-    </row>
-    <row r="1000" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A1000" s="20"/>
-      <c r="B1000" s="10"/>
-      <c r="C1000" s="10"/>
-      <c r="D1000" s="10"/>
-      <c r="E1000" s="10"/>
-      <c r="F1000" s="10"/>
-      <c r="G1000" s="10"/>
-      <c r="H1000" s="10"/>
-      <c r="I1000" s="10"/>
-      <c r="J1000" s="10"/>
-      <c r="K1000" s="10"/>
-      <c r="L1000" s="10"/>
-      <c r="M1000" s="10"/>
-      <c r="N1000" s="10"/>
-      <c r="O1000" s="10"/>
-      <c r="P1000" s="10"/>
-      <c r="Q1000" s="10"/>
-      <c r="R1000" s="10"/>
-      <c r="S1000" s="10"/>
-      <c r="T1000" s="10"/>
-      <c r="U1000" s="10"/>
-      <c r="V1000" s="10"/>
-      <c r="W1000" s="10"/>
-      <c r="X1000" s="10"/>
-      <c r="Y1000" s="10"/>
-      <c r="Z1000" s="21"/>
-    </row>
   </sheetData>
   <phoneticPr fontId="14" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>